<commit_message>
add changes to excel files
</commit_message>
<xml_diff>
--- a/6_Advanced_Data_Analysis/2_Data_Tables.xlsx
+++ b/6_Advanced_Data_Analysis/2_Data_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27920"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Developer\_Courses\Excel\Excel_Data_Analytics_Course\6_Advanced_Data_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\Excel_Data_Analytics_Course-main\Excel_Data_Analytics\Excel_Project-Data_Analytics\Excel_Project-Data_Analytics\6_Advanced_Data_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF699739-AF38-4398-A5C0-59458B85094B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F0D915-BE05-4610-AC3E-B9E0015566D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18336" windowHeight="10416" xr2:uid="{6C37AC85-509F-4D10-9DB1-F70D16D6FBAB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6C37AC85-509F-4D10-9DB1-F70D16D6FBAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="3" r:id="rId1"/>
@@ -468,6 +468,14 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="17" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="7" fillId="2" borderId="17" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="18" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -480,14 +488,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="17" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="7" fillId="2" borderId="17" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="18" xfId="3" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -831,20 +831,20 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5234375" customWidth="1"/>
-    <col min="3" max="3" width="11.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="11.05078125" customWidth="1"/>
+    <col min="6" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B2" s="22" t="s">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="23"/>
+      <c r="C2" s="29"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -852,11 +852,11 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="25">
         <v>100000</v>
       </c>
       <c r="E3" s="11"/>
@@ -867,11 +867,11 @@
       <c r="J3" s="20"/>
       <c r="K3" s="21"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="26">
         <v>0.1</v>
       </c>
       <c r="E4" s="16"/>
@@ -882,11 +882,11 @@
       <c r="J4" s="1"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="27">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E5" s="17"/>
@@ -897,7 +897,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" s="17"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -906,11 +906,11 @@
       <c r="J6" s="1"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="22" t="s">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="23"/>
+      <c r="C7" s="29"/>
       <c r="E7" s="17"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -919,7 +919,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
         <v>11</v>
       </c>
@@ -934,7 +934,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="9">
         <v>0</v>
       </c>
@@ -950,7 +950,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="9">
         <v>1</v>
       </c>
@@ -966,7 +966,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="9">
         <v>2</v>
       </c>
@@ -982,7 +982,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="9">
         <v>3</v>
       </c>
@@ -998,7 +998,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="9">
         <v>4</v>
       </c>
@@ -1007,11 +1007,11 @@
         <v>116749.99056874996</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="24">
         <f>SUM(C9:C13)</f>
         <v>566749.36181874992</v>
       </c>
@@ -1033,50 +1033,50 @@
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5234375" customWidth="1"/>
-    <col min="3" max="3" width="11.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="11.05078125" customWidth="1"/>
+    <col min="6" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B2" s="22" t="s">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="E2" s="26" t="s">
+      <c r="C2" s="29"/>
+      <c r="E2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="22" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="25">
         <v>100000</v>
       </c>
-      <c r="E3" s="27"/>
+      <c r="E3" s="23"/>
       <c r="F3" s="12">
         <f>C9</f>
         <v>110000.00000000001</v>
@@ -1102,11 +1102,11 @@
         <v>566749.36181874992</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="26">
         <v>0.1</v>
       </c>
       <c r="E4" s="17">
@@ -1132,11 +1132,11 @@
         <v>550000.00000000012</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="27">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E5" s="17">
@@ -1161,7 +1161,7 @@
         <v>555527.56881874998</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" s="17">
         <v>0.01</v>
       </c>
@@ -1184,11 +1184,11 @@
         <v>561110.55110000004</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="22" t="s">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="23"/>
+      <c r="C7" s="29"/>
       <c r="E7" s="17">
         <v>1.4999999999999999E-2</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>566749.36181874992</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
         <v>11</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>572444.41760000004</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="9">
         <v>0</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>578196.13671875</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="9">
         <v>1</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>584004.93910000008</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="9">
         <v>2</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>589871.24631874997</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="9">
         <v>3</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>595795.48160000006</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="9">
         <v>4</v>
       </c>
@@ -1369,11 +1369,11 @@
         <v>116749.99056874996</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="24">
         <f>SUM(C9:C13)</f>
         <v>566749.36181874992</v>
       </c>
@@ -1424,38 +1424,38 @@
       <selection activeCell="B2" sqref="B2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5234375" customWidth="1"/>
-    <col min="3" max="3" width="11.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="11.05078125" customWidth="1"/>
+    <col min="6" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B2" s="22" t="s">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="23"/>
+      <c r="C2" s="29"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-    </row>
-    <row r="3" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+    </row>
+    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="25">
         <v>100000</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="30" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="11">
@@ -1481,14 +1481,14 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="26">
         <v>0.1</v>
       </c>
-      <c r="D4" s="24"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="16">
         <v>0</v>
       </c>
@@ -1512,14 +1512,14 @@
         <v>625000</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="27">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D5" s="24"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1542,8 +1542,8 @@
         <v>631281.32820312493</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="D6" s="24"/>
+    <row r="6" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="30"/>
       <c r="E6" s="17">
         <v>0.01</v>
       </c>
@@ -1566,12 +1566,12 @@
         <v>637625.62624999997</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="22" t="s">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="17">
         <v>1.4999999999999999E-2</v>
       </c>
@@ -1594,14 +1594,14 @@
         <v>644033.3657031249</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="24"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="17">
         <v>0.02</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>650505.02</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="9">
         <v>0</v>
       </c>
@@ -1632,7 +1632,7 @@
         <f>(base*(1+raise)^B9)*(1+bonus)</f>
         <v>110000.00000000001</v>
       </c>
-      <c r="D9" s="24"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="17">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>657041.064453125</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="9">
         <v>1</v>
       </c>
@@ -1663,7 +1663,7 @@
         <f>(base*(1+raise)^B10)*(1+bonus)</f>
         <v>111650</v>
       </c>
-      <c r="D10" s="24"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="17">
         <v>0.03</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>663641.97625000007</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="9">
         <v>2</v>
       </c>
@@ -1694,7 +1694,7 @@
         <f>(base*(1+raise)^B11)*(1+bonus)</f>
         <v>113324.74999999997</v>
       </c>
-      <c r="D11" s="24"/>
+      <c r="D11" s="30"/>
       <c r="E11" s="17">
         <v>3.5000000000000003E-2</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>670308.23445312493</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="9">
         <v>3</v>
       </c>
@@ -1725,7 +1725,7 @@
         <f>(base*(1+raise)^B12)*(1+bonus)</f>
         <v>115024.62124999997</v>
       </c>
-      <c r="D12" s="24"/>
+      <c r="D12" s="30"/>
       <c r="E12" s="18">
         <v>0.04</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>677040.32000000007</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="9">
         <v>4</v>
       </c>
@@ -1757,11 +1757,11 @@
         <v>116749.99056874996</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="24">
         <f>SUM(C9:C13)</f>
         <v>566749.36181874992</v>
       </c>

</xml_diff>